<commit_message>
rename variables in excel spreadsheets and highligh difference
</commit_message>
<xml_diff>
--- a/docs/10-31-2013-energy-cost-calculator-generic-combined-heat-power-model.xlsx
+++ b/docs/10-31-2013-energy-cost-calculator-generic-combined-heat-power-model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr date1904="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omkai\Documents\Github\technoeconomic-assessment\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ADAF7F2C-21AC-4762-8927-CE50F4C0B045}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD2B81F-2E1D-4820-B5C9-188397D03169}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CHP_EconomicExample" sheetId="1" r:id="rId1"/>
@@ -631,9 +631,6 @@
     <t>Income--Capacity</t>
   </si>
   <si>
-    <t>Income--Heat sales</t>
-  </si>
-  <si>
     <t>Conventional</t>
   </si>
   <si>
@@ -727,25 +724,28 @@
     <t>Interest Rate on Debt:  Interest rate applied to debt portion of investment.  Value must be non-zero.</t>
   </si>
   <si>
-    <t>differences from generic-power-only are hightlighted in:</t>
-  </si>
-  <si>
     <t>Diff</t>
+  </si>
+  <si>
+    <t>different variables from generic-power-only are hightlighted in:</t>
+  </si>
+  <si>
+    <t>Income--Heat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="#,##0.0"/>
-    <numFmt numFmtId="170" formatCode="0.00000"/>
-    <numFmt numFmtId="172" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="168" formatCode="0.00000"/>
+    <numFmt numFmtId="169" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="9"/>
       <name val="Helv"/>
@@ -783,11 +783,6 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Verdana"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1299,7 +1294,7 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="3" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1338,7 +1333,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1387,7 +1382,7 @@
     <xf numFmtId="164" fontId="3" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1411,7 +1406,7 @@
     <xf numFmtId="3" fontId="3" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="5" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="169" fontId="5" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1451,7 +1446,7 @@
     <xf numFmtId="4" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1478,7 +1473,7 @@
     <xf numFmtId="2" fontId="3" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="3" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="3" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="3" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1488,10 +1483,10 @@
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="5" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4624,7 +4619,7 @@
 </file>
 
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor indexed="12"/>
   </sheetPr>
@@ -4639,7 +4634,7 @@
 </file>
 
 <file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor indexed="13"/>
   </sheetPr>
@@ -5702,14 +5697,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor indexed="52"/>
   </sheetPr>
   <dimension ref="A1:BD251"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="A162" sqref="A162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="12"/>
@@ -5720,7 +5715,7 @@
     <col min="4" max="4" width="13.83203125" style="2" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" style="2" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.5" style="2" customWidth="1"/>
     <col min="8" max="8" width="13.33203125" style="2" customWidth="1"/>
     <col min="9" max="9" width="11.33203125" style="2" customWidth="1"/>
     <col min="10" max="11" width="11.1640625" style="2" customWidth="1"/>
@@ -5774,8 +5769,8 @@
       <c r="E6" s="30"/>
       <c r="F6" s="30"/>
       <c r="G6" s="30"/>
-      <c r="H6" s="136" t="s">
-        <v>223</v>
+      <c r="H6" s="137" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -5793,7 +5788,7 @@
     </row>
     <row r="10" spans="1:9" ht="12.75" thickBot="1">
       <c r="B10" s="88" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C10" s="89"/>
       <c r="D10" s="90" t="s">
@@ -5890,7 +5885,7 @@
     </row>
     <row r="18" spans="1:9" ht="12.75" thickBot="1">
       <c r="B18" s="97" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C18" s="86"/>
       <c r="D18" s="87"/>
@@ -5949,7 +5944,7 @@
       <c r="A24" s="17"/>
       <c r="B24" s="31"/>
       <c r="D24" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -6443,7 +6438,7 @@
         <v>166</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -6508,7 +6503,7 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B80" s="14">
         <v>2.1</v>
@@ -6518,8 +6513,8 @@
       </c>
     </row>
     <row r="81" spans="1:4">
-      <c r="A81" s="11" t="s">
-        <v>194</v>
+      <c r="A81" s="134" t="s">
+        <v>193</v>
       </c>
       <c r="B81" s="14">
         <v>2.1</v>
@@ -6579,7 +6574,7 @@
         <v>5</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -7115,7 +7110,7 @@
         <v>123</v>
       </c>
       <c r="B124" s="99" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D124" s="2" t="s">
         <v>181</v>
@@ -8660,7 +8655,7 @@
     </row>
     <row r="161" spans="1:35">
       <c r="A161" s="132" t="s">
-        <v>190</v>
+        <v>223</v>
       </c>
       <c r="B161" s="44">
         <f>TotalIncomeFromHeatSales</f>
@@ -9154,7 +9149,7 @@
       <c r="AH165" s="4"/>
     </row>
     <row r="166" spans="1:35">
-      <c r="A166" s="137" t="s">
+      <c r="A166" s="136" t="s">
         <v>41</v>
       </c>
       <c r="B166" s="61">
@@ -9796,7 +9791,7 @@
     </row>
     <row r="186" spans="1:56" s="3" customFormat="1" ht="15">
       <c r="A186" s="100" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B186" s="10"/>
       <c r="C186" s="10"/>
@@ -9822,7 +9817,7 @@
     </row>
     <row r="187" spans="1:56">
       <c r="A187" s="11" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B187" s="4"/>
       <c r="C187" s="4"/>
@@ -9875,7 +9870,7 @@
       <c r="F189" s="139"/>
       <c r="G189" s="140"/>
       <c r="I189" s="138" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J189" s="139"/>
       <c r="K189" s="139"/>
@@ -9883,7 +9878,7 @@
       <c r="M189" s="139"/>
       <c r="N189" s="140"/>
       <c r="P189" s="138" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="Q189" s="139"/>
       <c r="R189" s="139"/>
@@ -9891,7 +9886,7 @@
       <c r="T189" s="139"/>
       <c r="U189" s="140"/>
       <c r="W189" s="138" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="X189" s="139"/>
       <c r="Y189" s="139"/>
@@ -9899,7 +9894,7 @@
       <c r="AA189" s="139"/>
       <c r="AB189" s="140"/>
       <c r="AD189" s="138" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AE189" s="139"/>
       <c r="AF189" s="139"/>
@@ -9907,7 +9902,7 @@
       <c r="AH189" s="139"/>
       <c r="AI189" s="140"/>
       <c r="AK189" s="138" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AL189" s="139"/>
       <c r="AM189" s="139"/>
@@ -9915,7 +9910,7 @@
       <c r="AO189" s="139"/>
       <c r="AP189" s="140"/>
       <c r="AR189" s="102" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AS189" s="101"/>
       <c r="AT189" s="101"/>
@@ -9926,7 +9921,7 @@
         <v>1.0200000000000001E-2</v>
       </c>
       <c r="AY189" s="138" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AZ189" s="139"/>
       <c r="BA189" s="139"/>
@@ -9937,285 +9932,285 @@
     <row r="190" spans="1:56" ht="36">
       <c r="A190" s="108"/>
       <c r="B190" s="109" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C190" s="110" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D190" s="110" t="s">
         <v>129</v>
       </c>
       <c r="E190" s="110" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F190" s="110" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G190" s="103" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I190" s="109" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J190" s="110" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K190" s="110" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L190" s="110" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="M190" s="110" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="N190" s="103" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="P190" s="109" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="Q190" s="110" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="R190" s="110" t="s">
+        <v>209</v>
+      </c>
+      <c r="S190" s="110" t="s">
+        <v>204</v>
+      </c>
+      <c r="T190" s="110" t="s">
+        <v>202</v>
+      </c>
+      <c r="U190" s="103" t="s">
+        <v>218</v>
+      </c>
+      <c r="W190" s="109" t="s">
+        <v>197</v>
+      </c>
+      <c r="X190" s="110" t="s">
+        <v>200</v>
+      </c>
+      <c r="Y190" s="110" t="s">
         <v>210</v>
       </c>
-      <c r="S190" s="110" t="s">
-        <v>205</v>
-      </c>
-      <c r="T190" s="110" t="s">
-        <v>203</v>
-      </c>
-      <c r="U190" s="103" t="s">
-        <v>219</v>
-      </c>
-      <c r="W190" s="109" t="s">
-        <v>198</v>
-      </c>
-      <c r="X190" s="110" t="s">
-        <v>201</v>
-      </c>
-      <c r="Y190" s="110" t="s">
+      <c r="Z190" s="110" t="s">
+        <v>204</v>
+      </c>
+      <c r="AA190" s="110" t="s">
+        <v>202</v>
+      </c>
+      <c r="AB190" s="103" t="s">
+        <v>218</v>
+      </c>
+      <c r="AD190" s="109" t="s">
+        <v>197</v>
+      </c>
+      <c r="AE190" s="110" t="s">
+        <v>200</v>
+      </c>
+      <c r="AF190" s="110" t="s">
+        <v>213</v>
+      </c>
+      <c r="AG190" s="110" t="s">
+        <v>204</v>
+      </c>
+      <c r="AH190" s="110" t="s">
+        <v>202</v>
+      </c>
+      <c r="AI190" s="103" t="s">
+        <v>218</v>
+      </c>
+      <c r="AK190" s="109" t="s">
+        <v>197</v>
+      </c>
+      <c r="AL190" s="110" t="s">
+        <v>200</v>
+      </c>
+      <c r="AM190" s="110" t="s">
+        <v>214</v>
+      </c>
+      <c r="AN190" s="110" t="s">
+        <v>204</v>
+      </c>
+      <c r="AO190" s="110" t="s">
+        <v>202</v>
+      </c>
+      <c r="AP190" s="103" t="s">
+        <v>218</v>
+      </c>
+      <c r="AR190" s="109" t="s">
+        <v>197</v>
+      </c>
+      <c r="AS190" s="110" t="s">
+        <v>200</v>
+      </c>
+      <c r="AT190" s="110" t="s">
         <v>211</v>
       </c>
-      <c r="Z190" s="110" t="s">
-        <v>205</v>
-      </c>
-      <c r="AA190" s="110" t="s">
-        <v>203</v>
-      </c>
-      <c r="AB190" s="103" t="s">
-        <v>219</v>
-      </c>
-      <c r="AD190" s="109" t="s">
-        <v>198</v>
-      </c>
-      <c r="AE190" s="110" t="s">
-        <v>201</v>
-      </c>
-      <c r="AF190" s="110" t="s">
-        <v>214</v>
-      </c>
-      <c r="AG190" s="110" t="s">
-        <v>205</v>
-      </c>
-      <c r="AH190" s="110" t="s">
-        <v>203</v>
-      </c>
-      <c r="AI190" s="103" t="s">
-        <v>219</v>
-      </c>
-      <c r="AK190" s="109" t="s">
-        <v>198</v>
-      </c>
-      <c r="AL190" s="110" t="s">
-        <v>201</v>
-      </c>
-      <c r="AM190" s="110" t="s">
+      <c r="AU190" s="110" t="s">
+        <v>204</v>
+      </c>
+      <c r="AV190" s="110" t="s">
+        <v>202</v>
+      </c>
+      <c r="AW190" s="103" t="s">
+        <v>218</v>
+      </c>
+      <c r="AY190" s="109" t="s">
+        <v>197</v>
+      </c>
+      <c r="AZ190" s="110" t="s">
+        <v>200</v>
+      </c>
+      <c r="BA190" s="110" t="s">
         <v>215</v>
       </c>
-      <c r="AN190" s="110" t="s">
-        <v>205</v>
-      </c>
-      <c r="AO190" s="110" t="s">
-        <v>203</v>
-      </c>
-      <c r="AP190" s="103" t="s">
-        <v>219</v>
-      </c>
-      <c r="AR190" s="109" t="s">
-        <v>198</v>
-      </c>
-      <c r="AS190" s="110" t="s">
-        <v>201</v>
-      </c>
-      <c r="AT190" s="110" t="s">
-        <v>212</v>
-      </c>
-      <c r="AU190" s="110" t="s">
-        <v>205</v>
-      </c>
-      <c r="AV190" s="110" t="s">
-        <v>203</v>
-      </c>
-      <c r="AW190" s="103" t="s">
-        <v>219</v>
-      </c>
-      <c r="AY190" s="109" t="s">
-        <v>198</v>
-      </c>
-      <c r="AZ190" s="110" t="s">
-        <v>201</v>
-      </c>
-      <c r="BA190" s="110" t="s">
+      <c r="BB190" s="110" t="s">
         <v>216</v>
       </c>
-      <c r="BB190" s="110" t="s">
+      <c r="BC190" s="110" t="s">
         <v>217</v>
       </c>
-      <c r="BC190" s="110" t="s">
+      <c r="BD190" s="103" t="s">
         <v>218</v>
-      </c>
-      <c r="BD190" s="103" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="191" spans="1:56">
       <c r="A191" s="108"/>
       <c r="B191" s="109"/>
       <c r="C191" s="110" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D191" s="110" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E191" s="110" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F191" s="110" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G191" s="90" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I191" s="109"/>
       <c r="J191" s="110" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K191" s="110" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="L191" s="110" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="M191" s="110" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="N191" s="90" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="P191" s="109"/>
       <c r="Q191" s="110" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="R191" s="110" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="S191" s="110" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="T191" s="110" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="U191" s="90" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="W191" s="109"/>
       <c r="X191" s="110" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="Y191" s="110" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="Z191" s="110" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AA191" s="110" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AB191" s="90" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AD191" s="109"/>
       <c r="AE191" s="110" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AF191" s="110" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AG191" s="110" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AH191" s="110" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AI191" s="90" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AK191" s="109"/>
       <c r="AL191" s="110" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AM191" s="110" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AN191" s="110" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AO191" s="110" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AP191" s="90" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AR191" s="109"/>
       <c r="AS191" s="110" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AT191" s="110" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AU191" s="110" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AV191" s="110" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AW191" s="90" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AY191" s="109"/>
       <c r="AZ191" s="110" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="BA191" s="110" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="BB191" s="110" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="BC191" s="110" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="BD191" s="90" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="192" spans="1:56" ht="21" customHeight="1">
       <c r="A192" s="108"/>
       <c r="B192" s="111" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C192" s="112"/>
       <c r="D192" s="112"/>
@@ -10229,7 +10224,7 @@
       </c>
       <c r="G192" s="104"/>
       <c r="I192" s="111" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J192" s="112"/>
       <c r="K192" s="112"/>
@@ -10243,7 +10238,7 @@
       </c>
       <c r="N192" s="104"/>
       <c r="P192" s="111" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="Q192" s="112"/>
       <c r="R192" s="112"/>
@@ -10257,7 +10252,7 @@
       </c>
       <c r="U192" s="104"/>
       <c r="W192" s="111" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="X192" s="112"/>
       <c r="Y192" s="112"/>
@@ -10271,7 +10266,7 @@
       </c>
       <c r="AB192" s="104"/>
       <c r="AD192" s="111" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AE192" s="112"/>
       <c r="AF192" s="112"/>
@@ -10285,7 +10280,7 @@
       </c>
       <c r="AI192" s="104"/>
       <c r="AK192" s="111" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AL192" s="112"/>
       <c r="AM192" s="112"/>
@@ -10299,7 +10294,7 @@
       </c>
       <c r="AP192" s="104"/>
       <c r="AR192" s="111" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AS192" s="112"/>
       <c r="AT192" s="112"/>
@@ -10313,7 +10308,7 @@
       </c>
       <c r="AW192" s="104"/>
       <c r="AY192" s="111" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AZ192" s="112"/>
       <c r="BA192" s="112"/>
@@ -10362,7 +10357,7 @@
         <v>0</v>
       </c>
       <c r="L193" s="116">
-        <f t="dataTable" ref="L193:M213" dt2D="0" dtr="0" r1="B54"/>
+        <f t="dataTable" ref="L193:M213" dt2D="0" dtr="0" r1="B54" ca="1"/>
         <v>2.9236190441176872E-2</v>
       </c>
       <c r="M193" s="116">
@@ -10428,7 +10423,7 @@
         <v>1</v>
       </c>
       <c r="AG193" s="116">
-        <f t="dataTable" ref="AG193:AH213" dt2D="0" dtr="0" r1="B87" ca="1"/>
+        <f t="dataTable" ref="AG193:AH213" dt2D="0" dtr="0" r1="B87"/>
         <v>4.6464398898748593E-2</v>
       </c>
       <c r="AH193" s="116">
@@ -12101,7 +12096,7 @@
     </row>
     <row r="203" spans="2:56">
       <c r="B203" s="114" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C203" s="115">
         <f>IF(ISERROR((D203-D203)/D203*100),"error",(D203-D203)/D203*100)</f>
@@ -12121,7 +12116,7 @@
         <v>0</v>
       </c>
       <c r="I203" s="114" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J203" s="115">
         <f t="shared" si="38"/>
@@ -12141,7 +12136,7 @@
         <v>0</v>
       </c>
       <c r="P203" s="114" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="Q203" s="115" t="str">
         <f t="shared" si="39"/>
@@ -12161,7 +12156,7 @@
         <v>0</v>
       </c>
       <c r="W203" s="114" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="X203" s="115">
         <f t="shared" si="40"/>
@@ -12181,7 +12176,7 @@
         <v>0</v>
       </c>
       <c r="AD203" s="114" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AE203" s="115">
         <f t="shared" si="41"/>
@@ -12201,7 +12196,7 @@
         <v>0</v>
       </c>
       <c r="AK203" s="114" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AL203" s="115">
         <f t="shared" si="42"/>
@@ -12221,7 +12216,7 @@
         <v>0</v>
       </c>
       <c r="AR203" s="114" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AS203" s="115">
         <f t="shared" si="43"/>
@@ -12241,7 +12236,7 @@
         <v>0</v>
       </c>
       <c r="AY203" s="114" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AZ203" s="115">
         <f t="shared" si="44"/>

</xml_diff>